<commit_message>
Fix issues in RSD heating (#1)
* Correct efficiency of RSD heating; use RSDAHT3 to account for ambient heat for cooling

* Do not apply both NCAP_AFA and NCAP_AFC to heating tech in RSD

* Check topology when specifying NCAP_AFC

* Define RSD space heating commodity groups

* Use defined RSD commodity groups to specify NCAP_AFC

* Adjust commodity filter when specifying COM_FR for RSD space heating

- this is to ensure predefined commodity groups does not cause Veda info messages

* Fix broken FLO_SHAR specification for ambient heat

* Calculate ambient heat share for existing HPs in SRV

* Adjust filter in LED space heating to exclude space heating CGs

* Increase the amount of ambient heat available in SRV in 2018-2021
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_A_SYS_SAD_1TS.xlsx
+++ b/SuppXLS/Scen_A_SYS_SAD_1TS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EEBEBB-8212-4149-8336-90BC2DB6B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FC455A-0DE4-4950-AEC7-BB7948EE7476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="12" r:id="rId1"/>
@@ -235,9 +235,6 @@
     <t>COM_FR</t>
   </si>
   <si>
-    <t>RSDSH*</t>
-  </si>
-  <si>
     <t>NCAP_AF</t>
   </si>
   <si>
@@ -383,6 +380,9 @@
   </si>
   <si>
     <t>Hour</t>
+  </si>
+  <si>
+    <t>RSDSH*-*</t>
   </si>
 </sst>
 </file>
@@ -612,6 +612,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -621,11 +626,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2128,12 +2128,12 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
@@ -2215,13 +2215,13 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+        <v>66</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
@@ -2247,13 +2247,13 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+        <v>67</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
@@ -2279,10 +2279,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -2339,13 +2339,13 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+        <v>69</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2371,9 +2371,9 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2427,13 +2427,13 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+        <v>70</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="13">
         <v>1</v>
@@ -2547,13 +2547,13 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="2"/>
@@ -2579,13 +2579,13 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="2"/>
@@ -2612,7 +2612,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -4581,7 +4581,7 @@
         <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4644,7 +4644,7 @@
         <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4713,7 +4713,7 @@
         <v>2018</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -4727,16 +4727,16 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>2018</v>
       </c>
       <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
         <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
       </c>
       <c r="H4">
         <v>0.59001999999999999</v>
@@ -4750,16 +4750,16 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>2018</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5">
         <v>7.3020000000000002E-2</v>
@@ -4830,13 +4830,13 @@
         <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3">
         <v>0.10802</v>
@@ -4858,144 +4858,144 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E87912A-05C7-48D9-8B04-811783F0B11F}">
   <dimension ref="B3:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="L4" t="s">
         <v>85</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" t="s">
         <v>86</v>
       </c>
-      <c r="M4" t="s">
-        <v>83</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>87</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
+        <v>89</v>
+      </c>
+      <c r="S4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="R4" t="s">
-        <v>90</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="C5" s="20" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>89</v>
+      <c r="D5" s="20" t="s">
+        <v>88</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R6">
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="L7">
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O7">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R7">
         <v>2</v>
       </c>
       <c r="S7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="L8">
         <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R8">
         <v>3</v>
       </c>
       <c r="S8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
@@ -5003,19 +5003,19 @@
         <v>4</v>
       </c>
       <c r="M9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O9">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R9">
         <v>4</v>
       </c>
       <c r="S9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
@@ -5023,124 +5023,124 @@
         <v>5</v>
       </c>
       <c r="M10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O10">
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R10">
         <v>5</v>
       </c>
       <c r="S10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
+      <c r="B11" s="21"/>
       <c r="L11">
         <v>6</v>
       </c>
       <c r="M11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O11">
         <v>6</v>
       </c>
       <c r="P11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R11">
         <v>6</v>
       </c>
       <c r="S11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
+      <c r="B12" s="21"/>
       <c r="L12">
         <v>7</v>
       </c>
       <c r="M12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R12">
         <v>7</v>
       </c>
       <c r="S12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
+      <c r="B13" s="21"/>
       <c r="L13">
         <v>8</v>
       </c>
       <c r="M13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R13">
         <v>8</v>
       </c>
       <c r="S13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
+      <c r="B14" s="21"/>
       <c r="L14">
         <v>9</v>
       </c>
       <c r="M14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R14">
         <v>9</v>
       </c>
       <c r="S14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
+      <c r="B15" s="21"/>
       <c r="L15">
         <v>10</v>
       </c>
       <c r="M15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R15">
         <v>10</v>
       </c>
       <c r="S15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
+      <c r="B16" s="21"/>
       <c r="L16">
         <v>11</v>
       </c>
       <c r="M16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R16">
         <v>11</v>
       </c>
       <c r="S16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
+      <c r="B17" s="21"/>
       <c r="R17">
         <v>12</v>
       </c>
       <c r="S17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -5148,7 +5148,7 @@
         <v>13</v>
       </c>
       <c r="S18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -5156,7 +5156,7 @@
         <v>14</v>
       </c>
       <c r="S19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
@@ -5164,7 +5164,7 @@
         <v>15</v>
       </c>
       <c r="S20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>16</v>
       </c>
       <c r="S21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -5180,7 +5180,7 @@
         <v>17</v>
       </c>
       <c r="S22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -5188,7 +5188,7 @@
         <v>18</v>
       </c>
       <c r="S23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>19</v>
       </c>
       <c r="S24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -5204,7 +5204,7 @@
         <v>20</v>
       </c>
       <c r="S25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -5212,7 +5212,7 @@
         <v>21</v>
       </c>
       <c r="S26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -5220,7 +5220,7 @@
         <v>22</v>
       </c>
       <c r="S27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
@@ -5228,7 +5228,7 @@
         <v>23</v>
       </c>
       <c r="S28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5507,7 +5507,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -5533,7 +5533,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5573,7 +5575,7 @@
         <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -5615,7 +5617,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>33</v>
@@ -5635,16 +5637,16 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>2018</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -5707,7 +5709,7 @@
         <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -5764,13 +5766,13 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3">
         <v>0.29060000000000002</v>
@@ -5784,13 +5786,13 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>2018</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4">
         <v>0.28925000000000001</v>
@@ -5804,13 +5806,13 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>2018</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5">
         <v>0.10802</v>
@@ -5824,13 +5826,13 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6">
         <v>2018</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>0.43824999999999997</v>
@@ -5844,13 +5846,13 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7">
         <v>2018</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7">
         <v>0.44740999999999997</v>
@@ -5893,10 +5895,10 @@
         <v>33</v>
       </c>
       <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
         <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -5991,10 +5993,10 @@
         <v>2018</v>
       </c>
       <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
       </c>
       <c r="G3">
         <v>1</v>

</xml_diff>